<commit_message>
got dropdown to connect with labels but not the correct label. Posted a question to StackOverflow to get issue resolved
</commit_message>
<xml_diff>
--- a/sample_data.xlsx
+++ b/sample_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8988" windowHeight="5388"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8985" windowHeight="5385"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="hh:mm:ss"/>
-    <numFmt numFmtId="166" formatCode="0.00000"/>
+    <numFmt numFmtId="165" formatCode="0.00000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -87,13 +87,13 @@
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -120,10 +120,10 @@
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="166" formatCode="0.00000"/>
+      <numFmt numFmtId="165" formatCode="0.00000"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="166" formatCode="0.00000"/>
+      <numFmt numFmtId="165" formatCode="0.00000"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="hh:mm:ss"/>
@@ -443,18 +443,18 @@
       <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="1"/>
-    <col min="2" max="2" width="16.44140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="14.109375" style="4" customWidth="1"/>
-    <col min="5" max="5" width="12" style="4" customWidth="1"/>
-    <col min="6" max="6" width="15" style="3" customWidth="1"/>
-    <col min="7" max="7" width="12.88671875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="1"/>
+    <col min="2" max="2" width="20.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -477,517 +477,517 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <f ca="1">NOW()</f>
-        <v>43741.393566550927</v>
+        <v>43776.69317337963</v>
       </c>
       <c r="B2" s="2">
         <f ca="1">RAND()/100</f>
-        <v>4.5605171362499974E-3</v>
+        <v>2.3212941819418796E-4</v>
       </c>
       <c r="C2" s="2">
         <f ca="1">B2+I2*RAND()/10000</f>
-        <v>4.5794965621371976E-3</v>
+        <v>2.0757256042067766E-4</v>
       </c>
       <c r="D2" s="4">
         <f ca="1">F2*$J$2</f>
-        <v>33.113914926311232</v>
+        <v>1.685491705507999</v>
       </c>
       <c r="E2" s="4">
         <f ca="1">G2*$J$2</f>
-        <v>33.338752023481199</v>
+        <v>1.2049082890958847</v>
       </c>
       <c r="F2" s="3">
         <f ca="1">B2*100</f>
-        <v>0.45605171362499974</v>
+        <v>2.3212941819418798E-2</v>
       </c>
       <c r="G2" s="3">
         <f ca="1">F2+I2*RAND()/100</f>
-        <v>0.45914821682249279</v>
+        <v>1.659424719867628E-2</v>
       </c>
       <c r="I2">
         <f ca="1">IF(RAND()&lt;0.5,1,-1)</f>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="J2">
         <v>72.61</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <f ca="1">A2-TIME(0,RANDBETWEEN(1,5),RANDBETWEEN(0,59))</f>
-        <v>43741.390962384263</v>
+        <v>43776.691437268521</v>
       </c>
       <c r="B3" s="2">
         <f t="shared" ref="B3:B16" ca="1" si="0">RAND()/100</f>
-        <v>5.6704509848814035E-3</v>
+        <v>6.6586698009037711E-4</v>
       </c>
       <c r="C3" s="2">
         <f t="shared" ref="C3:C16" ca="1" si="1">B3+I3*RAND()/10000</f>
-        <v>5.6923605201241092E-3</v>
+        <v>7.36206402322937E-4</v>
       </c>
       <c r="D3" s="4">
         <f t="shared" ref="D3:D16" ca="1" si="2">F3*$J$2</f>
-        <v>41.173144601223868</v>
+        <v>4.8348601424362281</v>
       </c>
       <c r="E3" s="4">
         <f t="shared" ref="E3:E16" ca="1" si="3">G3*$J$2</f>
-        <v>41.860403926593442</v>
+        <v>4.8717624835639324</v>
       </c>
       <c r="F3" s="3">
         <f t="shared" ref="F3:F16" ca="1" si="4">B3*100</f>
-        <v>0.56704509848814033</v>
+        <v>6.6586698009037715E-2</v>
       </c>
       <c r="G3" s="3">
         <f t="shared" ref="G3:G16" ca="1" si="5">F3+I3*RAND()/100</f>
-        <v>0.57651017665050874</v>
+        <v>6.7094924715107182E-2</v>
       </c>
       <c r="I3">
         <f t="shared" ref="I3:I16" ca="1" si="6">IF(RAND()&lt;0.5,1,-1)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <f t="shared" ref="A4:A16" ca="1" si="7">A3-TIME(0,RANDBETWEEN(1,5),RANDBETWEEN(0,59))</f>
-        <v>43741.388705439822</v>
+        <v>43776.690580787043</v>
       </c>
       <c r="B4" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>3.7878759960587528E-3</v>
+        <v>7.9149348595586883E-3</v>
       </c>
       <c r="C4" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>3.8148652034517513E-3</v>
+        <v>7.9723479634380111E-3</v>
       </c>
       <c r="D4" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>27.503767607382603</v>
+        <v>57.470342015255639</v>
       </c>
       <c r="E4" s="4">
         <f t="shared" ca="1" si="3"/>
-        <v>27.971009928418621</v>
+        <v>58.037331137392037</v>
       </c>
       <c r="F4" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>0.37878759960587527</v>
+        <v>0.79149348595586888</v>
       </c>
       <c r="G4" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>0.38522255789035426</v>
+        <v>0.79930217790100588</v>
       </c>
       <c r="I4">
         <f t="shared" ca="1" si="6"/>
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <f t="shared" ca="1" si="7"/>
-        <v>43741.386749421305</v>
+        <v>43776.688381712971</v>
       </c>
       <c r="B5" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>8.2332987961351023E-3</v>
+        <v>8.3213633113930242E-3</v>
       </c>
       <c r="C5" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>8.3254069703212804E-3</v>
+        <v>8.4183932927807455E-3</v>
       </c>
       <c r="D5" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>59.781982558736978</v>
+        <v>60.421419004024749</v>
       </c>
       <c r="E5" s="4">
         <f t="shared" ca="1" si="3"/>
-        <v>60.014450032675633</v>
+        <v>60.637379969934848</v>
       </c>
       <c r="F5" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>0.82332987961351023</v>
+        <v>0.83213633113930241</v>
       </c>
       <c r="G5" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>0.8265314699445756</v>
+        <v>0.83511059041364621</v>
       </c>
       <c r="I5">
         <f t="shared" ca="1" si="6"/>
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <f t="shared" ca="1" si="7"/>
-        <v>43741.384376736118</v>
+        <v>43776.685360879637</v>
       </c>
       <c r="B6" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.5364862426516402E-3</v>
+        <v>7.3230528918655155E-3</v>
       </c>
       <c r="C6" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>1.5768964922089534E-3</v>
+        <v>7.3193488109898038E-3</v>
       </c>
       <c r="D6" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>11.156426607893559</v>
+        <v>53.17268704783551</v>
       </c>
       <c r="E6" s="4">
         <f t="shared" ca="1" si="3"/>
-        <v>11.543781208744612</v>
+        <v>52.503182963245081</v>
       </c>
       <c r="F6" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>0.15364862426516401</v>
+        <v>0.73230528918655158</v>
       </c>
       <c r="G6" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>0.15898335227578311</v>
+        <v>0.72308473988768873</v>
       </c>
       <c r="I6">
         <f t="shared" ca="1" si="6"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <f t="shared" ca="1" si="7"/>
+        <v>43776.684550694452</v>
+      </c>
+      <c r="B7" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>5.0310810958958665E-3</v>
+      </c>
+      <c r="C7" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>4.9843269088938108E-3</v>
+      </c>
+      <c r="D7" s="4">
+        <f t="shared" ca="1" si="2"/>
+        <v>36.530679837299886</v>
+      </c>
+      <c r="E7" s="4">
+        <f t="shared" ca="1" si="3"/>
+        <v>35.827855518149619</v>
+      </c>
+      <c r="F7" s="3">
+        <f t="shared" ca="1" si="4"/>
+        <v>0.50310810958958663</v>
+      </c>
+      <c r="G7" s="3">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.49342866710025646</v>
+      </c>
+      <c r="I7">
+        <f t="shared" ca="1" si="6"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <f t="shared" ca="1" si="7"/>
+        <v>43776.683462731489</v>
+      </c>
+      <c r="B8" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>5.6296648208847234E-3</v>
+      </c>
+      <c r="C8" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>5.543896952972271E-3</v>
+      </c>
+      <c r="D8" s="4">
+        <f t="shared" ca="1" si="2"/>
+        <v>40.876996264443974</v>
+      </c>
+      <c r="E8" s="4">
+        <f t="shared" ca="1" si="3"/>
+        <v>40.683826737179729</v>
+      </c>
+      <c r="F8" s="3">
+        <f t="shared" ca="1" si="4"/>
+        <v>0.56296648208847233</v>
+      </c>
+      <c r="G8" s="3">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.5603061112405967</v>
+      </c>
+      <c r="I8">
+        <f t="shared" ca="1" si="6"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <f t="shared" ca="1" si="7"/>
+        <v>43776.681819212972</v>
+      </c>
+      <c r="B9" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>9.17798361524985E-3</v>
+      </c>
+      <c r="C9" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>9.2760232805439644E-3</v>
+      </c>
+      <c r="D9" s="4">
+        <f t="shared" ca="1" si="2"/>
+        <v>66.641339030329164</v>
+      </c>
+      <c r="E9" s="4">
+        <f t="shared" ca="1" si="3"/>
+        <v>66.95302644433022</v>
+      </c>
+      <c r="F9" s="3">
+        <f t="shared" ca="1" si="4"/>
+        <v>0.91779836152498495</v>
+      </c>
+      <c r="G9" s="3">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.92209098532337441</v>
+      </c>
+      <c r="I9">
+        <f t="shared" ca="1" si="6"/>
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
-        <f t="shared" ca="1" si="7"/>
-        <v>43741.382270254639</v>
-      </c>
-      <c r="B7" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>8.6933248087044321E-3</v>
-      </c>
-      <c r="C7" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>8.6325806982753446E-3</v>
-      </c>
-      <c r="D7" s="4">
-        <f t="shared" ca="1" si="2"/>
-        <v>63.122231436002885</v>
-      </c>
-      <c r="E7" s="4">
-        <f t="shared" ca="1" si="3"/>
-        <v>63.008192238422005</v>
-      </c>
-      <c r="F7" s="3">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.86933248087044324</v>
-      </c>
-      <c r="G7" s="3">
-        <f t="shared" ca="1" si="5"/>
-        <v>0.86776190935714093</v>
-      </c>
-      <c r="I7">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <f t="shared" ca="1" si="7"/>
+        <v>43776.679735879639</v>
+      </c>
+      <c r="B10" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.2185701617244027E-3</v>
+      </c>
+      <c r="C10" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>1.2224665700077736E-3</v>
+      </c>
+      <c r="D10" s="4">
+        <f t="shared" ca="1" si="2"/>
+        <v>8.8480379442808879</v>
+      </c>
+      <c r="E10" s="4">
+        <f t="shared" ca="1" si="3"/>
+        <v>9.2666704051795303</v>
+      </c>
+      <c r="F10" s="3">
+        <f t="shared" ca="1" si="4"/>
+        <v>0.12185701617244027</v>
+      </c>
+      <c r="G10" s="3">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.12762250936757374</v>
+      </c>
+      <c r="I10">
+        <f t="shared" ca="1" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <f t="shared" ca="1" si="7"/>
+        <v>43776.677363194452</v>
+      </c>
+      <c r="B11" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>8.4965546575431743E-3</v>
+      </c>
+      <c r="C11" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>8.5682358136468864E-3</v>
+      </c>
+      <c r="D11" s="4">
+        <f t="shared" ca="1" si="2"/>
+        <v>61.693483368420985</v>
+      </c>
+      <c r="E11" s="4">
+        <f t="shared" ca="1" si="3"/>
+        <v>62.009989628757815</v>
+      </c>
+      <c r="F11" s="3">
+        <f t="shared" ca="1" si="4"/>
+        <v>0.84965546575431738</v>
+      </c>
+      <c r="G11" s="3">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.8540144557052447</v>
+      </c>
+      <c r="I11">
+        <f t="shared" ca="1" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <f t="shared" ca="1" si="7"/>
+        <v>43776.674249768526</v>
+      </c>
+      <c r="B12" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>5.0518177188785315E-3</v>
+      </c>
+      <c r="C12" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>5.0278756358713662E-3</v>
+      </c>
+      <c r="D12" s="4">
+        <f t="shared" ca="1" si="2"/>
+        <v>36.68124845677702</v>
+      </c>
+      <c r="E12" s="4">
+        <f t="shared" ca="1" si="3"/>
+        <v>36.103198170651126</v>
+      </c>
+      <c r="F12" s="3">
+        <f t="shared" ca="1" si="4"/>
+        <v>0.50518177188785318</v>
+      </c>
+      <c r="G12" s="3">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.4972207432950162</v>
+      </c>
+      <c r="I12">
         <f t="shared" ca="1" si="6"/>
         <v>-1</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="1">
-        <f t="shared" ca="1" si="7"/>
-        <v>43741.380846643529</v>
-      </c>
-      <c r="B8" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>9.4449260912138674E-3</v>
-      </c>
-      <c r="C8" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>9.4105240542975473E-3</v>
-      </c>
-      <c r="D8" s="4">
-        <f t="shared" ca="1" si="2"/>
-        <v>68.579608348303893</v>
-      </c>
-      <c r="E8" s="4">
-        <f t="shared" ca="1" si="3"/>
-        <v>68.28182462092586</v>
-      </c>
-      <c r="F8" s="3">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.94449260912138677</v>
-      </c>
-      <c r="G8" s="3">
-        <f t="shared" ca="1" si="5"/>
-        <v>0.94039146978275534</v>
-      </c>
-      <c r="I8">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <f t="shared" ca="1" si="7"/>
+        <v>43776.672293750009</v>
+      </c>
+      <c r="B13" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>4.2822362631989843E-3</v>
+      </c>
+      <c r="C13" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>4.2139707380247967E-3</v>
+      </c>
+      <c r="D13" s="4">
+        <f t="shared" ca="1" si="2"/>
+        <v>31.093317507087825</v>
+      </c>
+      <c r="E13" s="4">
+        <f t="shared" ca="1" si="3"/>
+        <v>30.528936899078726</v>
+      </c>
+      <c r="F13" s="3">
+        <f t="shared" ca="1" si="4"/>
+        <v>0.42822362631989841</v>
+      </c>
+      <c r="G13" s="3">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.42045085937307158</v>
+      </c>
+      <c r="I13">
         <f t="shared" ca="1" si="6"/>
         <v>-1</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="1">
-        <f t="shared" ca="1" si="7"/>
-        <v>43741.379145254643</v>
-      </c>
-      <c r="B9" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>2.1233316963687565E-3</v>
-      </c>
-      <c r="C9" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>2.0758588455587769E-3</v>
-      </c>
-      <c r="D9" s="4">
-        <f t="shared" ca="1" si="2"/>
-        <v>15.41751144733354</v>
-      </c>
-      <c r="E9" s="4">
-        <f t="shared" ca="1" si="3"/>
-        <v>15.013877095552715</v>
-      </c>
-      <c r="F9" s="3">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.21233316963687565</v>
-      </c>
-      <c r="G9" s="3">
-        <f t="shared" ca="1" si="5"/>
-        <v>0.2067742335153934</v>
-      </c>
-      <c r="I9">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <f t="shared" ca="1" si="7"/>
+        <v>43776.66987476853</v>
+      </c>
+      <c r="B14" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>4.6830842390602834E-3</v>
+      </c>
+      <c r="C14" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>4.6209710018108568E-3</v>
+      </c>
+      <c r="D14" s="4">
+        <f t="shared" ca="1" si="2"/>
+        <v>34.003874659816717</v>
+      </c>
+      <c r="E14" s="4">
+        <f t="shared" ca="1" si="3"/>
+        <v>33.774372661398722</v>
+      </c>
+      <c r="F14" s="3">
+        <f t="shared" ca="1" si="4"/>
+        <v>0.46830842390602834</v>
+      </c>
+      <c r="G14" s="3">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.46514767471971796</v>
+      </c>
+      <c r="I14">
         <f t="shared" ca="1" si="6"/>
         <v>-1</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="1">
-        <f t="shared" ca="1" si="7"/>
-        <v>43741.376679976864</v>
-      </c>
-      <c r="B10" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>3.784311701773577E-3</v>
-      </c>
-      <c r="C10" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>3.8828830547292517E-3</v>
-      </c>
-      <c r="D10" s="4">
-        <f t="shared" ca="1" si="2"/>
-        <v>27.477887266577945</v>
-      </c>
-      <c r="E10" s="4">
-        <f t="shared" ca="1" si="3"/>
-        <v>27.693636998656107</v>
-      </c>
-      <c r="F10" s="3">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.37843117017735772</v>
-      </c>
-      <c r="G10" s="3">
-        <f t="shared" ca="1" si="5"/>
-        <v>0.38140252029549798</v>
-      </c>
-      <c r="I10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <f t="shared" ca="1" si="7"/>
+        <v>43776.66809236112</v>
+      </c>
+      <c r="B15" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>6.6713578682811806E-3</v>
+      </c>
+      <c r="C15" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>6.7365509168717331E-3</v>
+      </c>
+      <c r="D15" s="4">
+        <f t="shared" ca="1" si="2"/>
+        <v>48.440729481589649</v>
+      </c>
+      <c r="E15" s="4">
+        <f t="shared" ca="1" si="3"/>
+        <v>48.841578568634468</v>
+      </c>
+      <c r="F15" s="3">
+        <f t="shared" ca="1" si="4"/>
+        <v>0.66713578682811803</v>
+      </c>
+      <c r="G15" s="3">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.67265636370519855</v>
+      </c>
+      <c r="I15">
         <f t="shared" ca="1" si="6"/>
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="1">
-        <f t="shared" ca="1" si="7"/>
-        <v>43741.372594328714</v>
-      </c>
-      <c r="B11" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>5.2918343660739824E-3</v>
-      </c>
-      <c r="C11" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>5.2012396281550227E-3</v>
-      </c>
-      <c r="D11" s="4">
-        <f t="shared" ca="1" si="2"/>
-        <v>38.424009332063186</v>
-      </c>
-      <c r="E11" s="4">
-        <f t="shared" ca="1" si="3"/>
-        <v>38.364966548985649</v>
-      </c>
-      <c r="F11" s="3">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.52918343660739819</v>
-      </c>
-      <c r="G11" s="3">
-        <f t="shared" ca="1" si="5"/>
-        <v>0.52837028713656042</v>
-      </c>
-      <c r="I11">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <f t="shared" ca="1" si="7"/>
+        <v>43776.664492824086</v>
+      </c>
+      <c r="B16" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>5.2050640945783457E-3</v>
+      </c>
+      <c r="C16" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>5.1494524896321635E-3</v>
+      </c>
+      <c r="D16" s="4">
+        <f t="shared" ca="1" si="2"/>
+        <v>37.793970390733364</v>
+      </c>
+      <c r="E16" s="4">
+        <f t="shared" ca="1" si="3"/>
+        <v>37.592054706253222</v>
+      </c>
+      <c r="F16" s="3">
+        <f t="shared" ca="1" si="4"/>
+        <v>0.52050640945783455</v>
+      </c>
+      <c r="G16" s="3">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.5177255847163369</v>
+      </c>
+      <c r="I16">
         <f t="shared" ca="1" si="6"/>
         <v>-1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="1">
-        <f t="shared" ca="1" si="7"/>
-        <v>43741.371066550935</v>
-      </c>
-      <c r="B12" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.3935322843095965E-3</v>
-      </c>
-      <c r="C12" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.4638991435755339E-3</v>
-      </c>
-      <c r="D12" s="4">
-        <f t="shared" ca="1" si="2"/>
-        <v>10.118437916371981</v>
-      </c>
-      <c r="E12" s="4">
-        <f t="shared" ca="1" si="3"/>
-        <v>10.521011449916557</v>
-      </c>
-      <c r="F12" s="3">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.13935322843095965</v>
-      </c>
-      <c r="G12" s="3">
-        <f t="shared" ca="1" si="5"/>
-        <v>0.14489755474337634</v>
-      </c>
-      <c r="I12">
-        <f t="shared" ca="1" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="1">
-        <f t="shared" ca="1" si="7"/>
-        <v>43741.369666087972</v>
-      </c>
-      <c r="B13" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>4.7114849958434617E-3</v>
-      </c>
-      <c r="C13" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>4.7382015084441662E-3</v>
-      </c>
-      <c r="D13" s="4">
-        <f t="shared" ca="1" si="2"/>
-        <v>34.210092554819376</v>
-      </c>
-      <c r="E13" s="4">
-        <f t="shared" ca="1" si="3"/>
-        <v>34.769479354147201</v>
-      </c>
-      <c r="F13" s="3">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.47114849958434618</v>
-      </c>
-      <c r="G13" s="3">
-        <f t="shared" ca="1" si="5"/>
-        <v>0.47885249076087594</v>
-      </c>
-      <c r="I13">
-        <f t="shared" ca="1" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="1">
-        <f t="shared" ca="1" si="7"/>
-        <v>43741.366587384269</v>
-      </c>
-      <c r="B14" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>3.8251787905497869E-3</v>
-      </c>
-      <c r="C14" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>3.894125544265097E-3</v>
-      </c>
-      <c r="D14" s="4">
-        <f t="shared" ca="1" si="2"/>
-        <v>27.774623198182002</v>
-      </c>
-      <c r="E14" s="4">
-        <f t="shared" ca="1" si="3"/>
-        <v>27.974303091931546</v>
-      </c>
-      <c r="F14" s="3">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.38251787905497869</v>
-      </c>
-      <c r="G14" s="3">
-        <f t="shared" ca="1" si="5"/>
-        <v>0.38526791202219457</v>
-      </c>
-      <c r="I14">
-        <f t="shared" ca="1" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" s="1">
-        <f t="shared" ca="1" si="7"/>
-        <v>43741.364816550937</v>
-      </c>
-      <c r="B15" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>8.3202849720241598E-3</v>
-      </c>
-      <c r="C15" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>8.373132249907992E-3</v>
-      </c>
-      <c r="D15" s="4">
-        <f t="shared" ca="1" si="2"/>
-        <v>60.413589181867422</v>
-      </c>
-      <c r="E15" s="4">
-        <f t="shared" ca="1" si="3"/>
-        <v>60.522686443571608</v>
-      </c>
-      <c r="F15" s="3">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.83202849720241601</v>
-      </c>
-      <c r="G15" s="3">
-        <f t="shared" ca="1" si="5"/>
-        <v>0.83353100734845897</v>
-      </c>
-      <c r="I15">
-        <f t="shared" ca="1" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="1">
-        <f t="shared" ca="1" si="7"/>
-        <v>43741.362351273157</v>
-      </c>
-      <c r="B16" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>4.8567067398822342E-3</v>
-      </c>
-      <c r="C16" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>4.8696855890025936E-3</v>
-      </c>
-      <c r="D16" s="4">
-        <f t="shared" ca="1" si="2"/>
-        <v>35.264547638284903</v>
-      </c>
-      <c r="E16" s="4">
-        <f t="shared" ca="1" si="3"/>
-        <v>35.791179031515291</v>
-      </c>
-      <c r="F16" s="3">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.48567067398822339</v>
-      </c>
-      <c r="G16" s="3">
-        <f t="shared" ca="1" si="5"/>
-        <v>0.49292355090917628</v>
-      </c>
-      <c r="I16">
-        <f t="shared" ca="1" si="6"/>
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>